<commit_message>
More Science Edits - Probably last big commit for the week.
</commit_message>
<xml_diff>
--- a/Plotting/0.9.0/SSSScienceExperiments.xlsx
+++ b/Plotting/0.9.0/SSSScienceExperiments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\Steam\steamapps\common\Kerbal Space Program\GameData\SkyhawkScienceSystem\Plotting\0.9.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B58D3480-E047-40B9-A06D-6CB9B867965E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74CBCD90-F81F-428C-ADFA-3EA814E74545}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1152" yWindow="1128" windowWidth="15228" windowHeight="11232" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="103">
   <si>
     <t>Tier</t>
   </si>
@@ -36,12 +36,6 @@
     <t>Base Value</t>
   </si>
   <si>
-    <t>Probes Before Crew</t>
-  </si>
-  <si>
-    <t>Source/Inspiration</t>
-  </si>
-  <si>
     <t>SSS_telemetryReport</t>
   </si>
   <si>
@@ -105,9 +99,6 @@
     <t>SSS_chargedParticlesScan</t>
   </si>
   <si>
-    <t>SSS_IRSpec</t>
-  </si>
-  <si>
     <t>SSS_ionElec</t>
   </si>
   <si>
@@ -117,15 +108,9 @@
     <t>Charged Particles Scan</t>
   </si>
   <si>
-    <t>IR Spectroscopy</t>
-  </si>
-  <si>
     <t>Ionization and Electrostatic Analysis</t>
   </si>
   <si>
-    <t>Gamma Ray Detection</t>
-  </si>
-  <si>
     <t>SSS_Geodesy</t>
   </si>
   <si>
@@ -136,6 +121,219 @@
   </si>
   <si>
     <t>SSS_basicWeatherImaging</t>
+  </si>
+  <si>
+    <t>Gamma Ray Spectrometry</t>
+  </si>
+  <si>
+    <t>Biological Experiments</t>
+  </si>
+  <si>
+    <t>X-Ray Imaging</t>
+  </si>
+  <si>
+    <t>Orbital Reconnaissance Camera</t>
+  </si>
+  <si>
+    <t>UV and Atmospheric Analysis</t>
+  </si>
+  <si>
+    <t>Coatl Aerospace/Bluedog_DB</t>
+  </si>
+  <si>
+    <t>Micrometeroid Impact Data</t>
+  </si>
+  <si>
+    <t>Transmissible Film Camera</t>
+  </si>
+  <si>
+    <t>Orbital Sun Observations</t>
+  </si>
+  <si>
+    <t>Solar Wind Observations</t>
+  </si>
+  <si>
+    <t>Advanced Weather Imaging</t>
+  </si>
+  <si>
+    <t>IR Spectrometry</t>
+  </si>
+  <si>
+    <t>Infrared Radiation Data</t>
+  </si>
+  <si>
+    <t>Microwave Spectrometry</t>
+  </si>
+  <si>
+    <t>Crew Report</t>
+  </si>
+  <si>
+    <t>Mystery Goo</t>
+  </si>
+  <si>
+    <t>Seismic Scan</t>
+  </si>
+  <si>
+    <t>Surface Material Exposure</t>
+  </si>
+  <si>
+    <t>Coatl Aerospace</t>
+  </si>
+  <si>
+    <t>Exclusive? (Not stock of BDB, and only part of that mod)</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Mass Spectrum Analysis</t>
+  </si>
+  <si>
+    <t>High Resolution Ultraviolet Imaging</t>
+  </si>
+  <si>
+    <t>Digital Camera</t>
+  </si>
+  <si>
+    <t>RPWS</t>
+  </si>
+  <si>
+    <t>Note - look at BDB's sciencedefs_compatability to get an idea how to make things work better!</t>
+  </si>
+  <si>
+    <t>Orbital Surveillance Camera</t>
+  </si>
+  <si>
+    <t>EVA Report</t>
+  </si>
+  <si>
+    <t>Science Jr/Mobile Materials Lab</t>
+  </si>
+  <si>
+    <t>Surface Sample</t>
+  </si>
+  <si>
+    <t>KDEX Dust Analysis</t>
+  </si>
+  <si>
+    <t>SIGINT Scan</t>
+  </si>
+  <si>
+    <t>Solar Wind Dust Collector</t>
+  </si>
+  <si>
+    <t>DMagicOrbitalScience</t>
+  </si>
+  <si>
+    <t>Atmospheric Analysis</t>
+  </si>
+  <si>
+    <t>Asteroid Survey Telescope</t>
+  </si>
+  <si>
+    <t>Skylab Solar Telescope</t>
+  </si>
+  <si>
+    <t>Hydrometer</t>
+  </si>
+  <si>
+    <t>Orbital Scope //could be retro fit to digital camera, same science defs!</t>
+  </si>
+  <si>
+    <t>Photopolarimeter</t>
+  </si>
+  <si>
+    <t>radarAltimeter</t>
+  </si>
+  <si>
+    <t>trappedRadiation</t>
+  </si>
+  <si>
+    <t>Antimatter Scanner</t>
+  </si>
+  <si>
+    <t>FarFutureTechnologies</t>
+  </si>
+  <si>
+    <t>Rational Resources Resource Report</t>
+  </si>
+  <si>
+    <t>RationalResources</t>
+  </si>
+  <si>
+    <t>Source - ideally all should be stock, BDB, and then a few customs</t>
+  </si>
+  <si>
+    <t>Multispectral Analysis</t>
+  </si>
+  <si>
+    <t>Recon Scan</t>
+  </si>
+  <si>
+    <t>Surface Hydrogen Scan</t>
+  </si>
+  <si>
+    <t>X-Ray Diffraction Scan</t>
+  </si>
+  <si>
+    <t>Laser Surface Scan</t>
+  </si>
+  <si>
+    <t>Soil Moisture Scan (Hydrometer?)</t>
+  </si>
+  <si>
+    <t>Asteroid Interior Scan</t>
+  </si>
+  <si>
+    <t>Irradiance Scan</t>
+  </si>
+  <si>
+    <t>Seismic Data</t>
+  </si>
+  <si>
+    <t>Bathymetry Data</t>
+  </si>
+  <si>
+    <t>Bio Drill Scan</t>
+  </si>
+  <si>
+    <t>Anomaly Scan</t>
+  </si>
+  <si>
+    <t>Student Experiments</t>
+  </si>
+  <si>
+    <t>Customer Experiments</t>
+  </si>
+  <si>
+    <t>KSC Experiments</t>
+  </si>
+  <si>
+    <t>Luciole</t>
+  </si>
+  <si>
+    <t>Plant Growth Study</t>
+  </si>
+  <si>
+    <t>KPBS</t>
+  </si>
+  <si>
+    <t>SCAN Altimetry</t>
+  </si>
+  <si>
+    <t>SCANSat</t>
+  </si>
+  <si>
+    <t>Fish Study</t>
+  </si>
+  <si>
+    <t>Telescope Observations</t>
+  </si>
+  <si>
+    <t>SSPX</t>
+  </si>
+  <si>
+    <t>Interkosmos/Bluedog_DB</t>
   </si>
 </sst>
 </file>
@@ -453,18 +651,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="D45" workbookViewId="0">
+      <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.44140625" customWidth="1"/>
-    <col min="2" max="2" width="24.77734375" customWidth="1"/>
-    <col min="3" max="3" width="25.33203125" customWidth="1"/>
+    <col min="1" max="1" width="4.6640625" customWidth="1"/>
+    <col min="2" max="2" width="24.77734375" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="30.33203125" customWidth="1"/>
     <col min="4" max="4" width="9.88671875" customWidth="1"/>
+    <col min="5" max="5" width="25.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -472,7 +671,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -481,7 +680,10 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>78</v>
+      </c>
+      <c r="G1" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -489,16 +691,19 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D2">
         <v>12</v>
       </c>
       <c r="E2" t="s">
-        <v>3</v>
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -506,16 +711,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D3">
         <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -523,16 +728,16 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D4">
         <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -540,16 +745,16 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D5">
         <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -557,13 +762,13 @@
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -571,13 +776,13 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E7" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -585,13 +790,13 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E8" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -599,13 +804,13 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E9" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -613,58 +818,49 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>2</v>
       </c>
-      <c r="B11" t="s">
-        <v>27</v>
-      </c>
       <c r="C11" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C12" t="s">
         <v>32</v>
       </c>
       <c r="E12" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>3</v>
-      </c>
-      <c r="B13" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="E13" t="s">
-        <v>14</v>
-      </c>
-      <c r="H13" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
@@ -672,13 +868,16 @@
         <v>3</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="E14" t="s">
-        <v>14</v>
+        <v>12</v>
+      </c>
+      <c r="H14" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
@@ -686,7 +885,615 @@
         <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>33</v>
+        <v>31</v>
+      </c>
+      <c r="C15" t="s">
+        <v>30</v>
+      </c>
+      <c r="E15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>3</v>
+      </c>
+      <c r="B16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>3</v>
+      </c>
+      <c r="C17" t="s">
+        <v>36</v>
+      </c>
+      <c r="E17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>4</v>
+      </c>
+      <c r="C18" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>4</v>
+      </c>
+      <c r="C19" t="s">
+        <v>39</v>
+      </c>
+      <c r="E19" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>4</v>
+      </c>
+      <c r="C20" t="s">
+        <v>40</v>
+      </c>
+      <c r="E20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>4</v>
+      </c>
+      <c r="C21" t="s">
+        <v>41</v>
+      </c>
+      <c r="E21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>4</v>
+      </c>
+      <c r="C22" t="s">
+        <v>42</v>
+      </c>
+      <c r="E22" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>4</v>
+      </c>
+      <c r="C23" t="s">
+        <v>43</v>
+      </c>
+      <c r="E23" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>4</v>
+      </c>
+      <c r="C24" t="s">
+        <v>44</v>
+      </c>
+      <c r="E24" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>4</v>
+      </c>
+      <c r="C25" t="s">
+        <v>45</v>
+      </c>
+      <c r="E25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>5</v>
+      </c>
+      <c r="C26" t="s">
+        <v>46</v>
+      </c>
+      <c r="E26" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>5</v>
+      </c>
+      <c r="C27" t="s">
+        <v>47</v>
+      </c>
+      <c r="E27" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>5</v>
+      </c>
+      <c r="C28" t="s">
+        <v>48</v>
+      </c>
+      <c r="E28" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>5</v>
+      </c>
+      <c r="C29" t="s">
+        <v>49</v>
+      </c>
+      <c r="E29" t="s">
+        <v>50</v>
+      </c>
+      <c r="G29" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>5</v>
+      </c>
+      <c r="C30" t="s">
+        <v>53</v>
+      </c>
+      <c r="E30" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>5</v>
+      </c>
+      <c r="C31" t="s">
+        <v>54</v>
+      </c>
+      <c r="E31" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>6</v>
+      </c>
+      <c r="C32" t="s">
+        <v>55</v>
+      </c>
+      <c r="E32" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>6</v>
+      </c>
+      <c r="C33" t="s">
+        <v>56</v>
+      </c>
+      <c r="E33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>6</v>
+      </c>
+      <c r="C34" t="s">
+        <v>58</v>
+      </c>
+      <c r="E34" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>6</v>
+      </c>
+      <c r="C35" t="s">
+        <v>59</v>
+      </c>
+      <c r="E35" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>7</v>
+      </c>
+      <c r="C36" t="s">
+        <v>60</v>
+      </c>
+      <c r="E36" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>7</v>
+      </c>
+      <c r="C37" t="s">
+        <v>61</v>
+      </c>
+      <c r="E37" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>7</v>
+      </c>
+      <c r="C38" t="s">
+        <v>62</v>
+      </c>
+      <c r="E38" t="s">
+        <v>50</v>
+      </c>
+      <c r="G38" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>7</v>
+      </c>
+      <c r="C39" t="s">
+        <v>63</v>
+      </c>
+      <c r="E39" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>7</v>
+      </c>
+      <c r="C40" t="s">
+        <v>64</v>
+      </c>
+      <c r="E40" t="s">
+        <v>65</v>
+      </c>
+      <c r="G40" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>8</v>
+      </c>
+      <c r="C41" t="s">
+        <v>66</v>
+      </c>
+      <c r="E41" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>8</v>
+      </c>
+      <c r="C42" t="s">
+        <v>76</v>
+      </c>
+      <c r="E42" t="s">
+        <v>77</v>
+      </c>
+      <c r="G42" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>9</v>
+      </c>
+      <c r="C43" t="s">
+        <v>68</v>
+      </c>
+      <c r="E43" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>10</v>
+      </c>
+      <c r="C44" t="s">
+        <v>67</v>
+      </c>
+      <c r="E44" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>11</v>
+      </c>
+      <c r="C45" t="s">
+        <v>74</v>
+      </c>
+      <c r="E45" t="s">
+        <v>75</v>
+      </c>
+      <c r="G45" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C46" t="s">
+        <v>69</v>
+      </c>
+      <c r="E46" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C47" t="s">
+        <v>70</v>
+      </c>
+      <c r="E47" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C48" t="s">
+        <v>71</v>
+      </c>
+      <c r="E48" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="49" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C49" t="s">
+        <v>72</v>
+      </c>
+      <c r="E49" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="50" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C50" t="s">
+        <v>73</v>
+      </c>
+      <c r="E50" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="51" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C51" t="s">
+        <v>79</v>
+      </c>
+      <c r="E51" t="s">
+        <v>65</v>
+      </c>
+      <c r="G51" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="52" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C52" t="s">
+        <v>80</v>
+      </c>
+      <c r="E52" t="s">
+        <v>65</v>
+      </c>
+      <c r="G52" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="53" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C53" t="s">
+        <v>81</v>
+      </c>
+      <c r="E53" t="s">
+        <v>65</v>
+      </c>
+      <c r="G53" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C54" t="s">
+        <v>82</v>
+      </c>
+      <c r="E54" t="s">
+        <v>65</v>
+      </c>
+      <c r="G54" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="55" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C55" t="s">
+        <v>83</v>
+      </c>
+      <c r="E55" t="s">
+        <v>65</v>
+      </c>
+      <c r="G55" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="56" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C56" t="s">
+        <v>84</v>
+      </c>
+      <c r="E56" t="s">
+        <v>65</v>
+      </c>
+      <c r="G56" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="57" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C57" t="s">
+        <v>85</v>
+      </c>
+      <c r="E57" t="s">
+        <v>65</v>
+      </c>
+      <c r="G57" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="58" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C58" t="s">
+        <v>86</v>
+      </c>
+      <c r="E58" t="s">
+        <v>65</v>
+      </c>
+      <c r="G58" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="59" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C59" t="s">
+        <v>87</v>
+      </c>
+      <c r="E59" t="s">
+        <v>65</v>
+      </c>
+      <c r="G59" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="60" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C60" t="s">
+        <v>88</v>
+      </c>
+      <c r="E60" t="s">
+        <v>65</v>
+      </c>
+      <c r="G60" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="61" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C61" t="s">
+        <v>89</v>
+      </c>
+      <c r="E61" t="s">
+        <v>65</v>
+      </c>
+      <c r="G61" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="62" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C62" t="s">
+        <v>90</v>
+      </c>
+      <c r="E62" t="s">
+        <v>65</v>
+      </c>
+      <c r="G62" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="63" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C63" t="s">
+        <v>91</v>
+      </c>
+      <c r="E63" t="s">
+        <v>94</v>
+      </c>
+      <c r="G63" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="64" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C64" t="s">
+        <v>92</v>
+      </c>
+      <c r="E64" t="s">
+        <v>94</v>
+      </c>
+      <c r="G64" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="65" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C65" t="s">
+        <v>93</v>
+      </c>
+      <c r="E65" t="s">
+        <v>94</v>
+      </c>
+      <c r="G65" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="66" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C66" t="s">
+        <v>95</v>
+      </c>
+      <c r="E66" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="67" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C67" t="s">
+        <v>97</v>
+      </c>
+      <c r="E67" t="s">
+        <v>98</v>
+      </c>
+      <c r="G67" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="68" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C68" t="s">
+        <v>99</v>
+      </c>
+      <c r="E68" t="s">
+        <v>101</v>
+      </c>
+      <c r="G68" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="69" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C69" t="s">
+        <v>95</v>
+      </c>
+      <c r="E69" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="70" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C70" t="s">
+        <v>100</v>
+      </c>
+      <c r="E70" t="s">
+        <v>101</v>
+      </c>
+      <c r="G70" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Back at work! Here are some wrap ups of science balancing, and a few localization changes.
</commit_message>
<xml_diff>
--- a/Plotting/0.9.0/SSSScienceExperiments.xlsx
+++ b/Plotting/0.9.0/SSSScienceExperiments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\Steam\steamapps\common\Kerbal Space Program\GameData\SkyhawkScienceSystem\Plotting\0.9.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74CBCD90-F81F-428C-ADFA-3EA814E74545}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B0F2A15-44F2-463F-952D-CB0281CC6142}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1128" windowWidth="15228" windowHeight="11232" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2304" yWindow="1728" windowWidth="15228" windowHeight="11232" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="110">
   <si>
     <t>Tier</t>
   </si>
@@ -72,9 +72,6 @@
     <t>Telemetry Report</t>
   </si>
   <si>
-    <t>Film Camera</t>
-  </si>
-  <si>
     <t>Temperature Scan</t>
   </si>
   <si>
@@ -135,18 +132,12 @@
     <t>Orbital Reconnaissance Camera</t>
   </si>
   <si>
-    <t>UV and Atmospheric Analysis</t>
-  </si>
-  <si>
     <t>Coatl Aerospace/Bluedog_DB</t>
   </si>
   <si>
     <t>Micrometeroid Impact Data</t>
   </si>
   <si>
-    <t>Transmissible Film Camera</t>
-  </si>
-  <si>
     <t>Orbital Sun Observations</t>
   </si>
   <si>
@@ -192,9 +183,6 @@
     <t>High Resolution Ultraviolet Imaging</t>
   </si>
   <si>
-    <t>Digital Camera</t>
-  </si>
-  <si>
     <t>RPWS</t>
   </si>
   <si>
@@ -237,9 +225,6 @@
     <t>Hydrometer</t>
   </si>
   <si>
-    <t>Orbital Scope //could be retro fit to digital camera, same science defs!</t>
-  </si>
-  <si>
     <t>Photopolarimeter</t>
   </si>
   <si>
@@ -334,6 +319,42 @@
   </si>
   <si>
     <t>Interkosmos/Bluedog_DB</t>
+  </si>
+  <si>
+    <t>DMagicOrbitalScience/Bluedog_DB</t>
+  </si>
+  <si>
+    <t>Film Camera Imagery</t>
+  </si>
+  <si>
+    <t>Digital Camera Imagery/Orbital Telescope</t>
+  </si>
+  <si>
+    <t>Hubble Telescope</t>
+  </si>
+  <si>
+    <t>ResearchBodies/SpaceDust/HullcamVDS</t>
+  </si>
+  <si>
+    <t>Geodesic Surveys</t>
+  </si>
+  <si>
+    <t>Needs multiple runs?</t>
+  </si>
+  <si>
+    <t>//High Science to make up for the fact that you will be launching a ton of them to harvest it all.</t>
+  </si>
+  <si>
+    <t>//Adds up to quite a bit of science when u figure in the fact its biome based.</t>
+  </si>
+  <si>
+    <t>Ultraviolet and Atmospheric Analysis</t>
+  </si>
+  <si>
+    <t>Cosmic Ray Data</t>
+  </si>
+  <si>
+    <t>Gravity Scan</t>
   </si>
 </sst>
 </file>
@@ -651,10 +672,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H70"/>
+  <dimension ref="A1:H72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D45" workbookViewId="0">
-      <selection activeCell="E48" sqref="E48"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="A72" sqref="A72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -663,7 +684,8 @@
     <col min="2" max="2" width="24.77734375" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="30.33203125" customWidth="1"/>
     <col min="4" max="4" width="9.88671875" customWidth="1"/>
-    <col min="5" max="5" width="25.44140625" customWidth="1"/>
+    <col min="5" max="5" width="19.109375" customWidth="1"/>
+    <col min="6" max="6" width="14.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -680,10 +702,13 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>78</v>
+        <v>73</v>
+      </c>
+      <c r="F1" t="s">
+        <v>104</v>
       </c>
       <c r="G1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -703,7 +728,7 @@
         <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -714,7 +739,7 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D3">
         <v>12</v>
@@ -731,7 +756,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D4">
         <v>12</v>
@@ -748,7 +773,7 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>99</v>
       </c>
       <c r="D5">
         <v>16</v>
@@ -765,10 +790,13 @@
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="D6">
+        <v>11</v>
       </c>
       <c r="E6" t="s">
-        <v>6</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
@@ -779,7 +807,10 @@
         <v>10</v>
       </c>
       <c r="C7" t="s">
-        <v>19</v>
+        <v>18</v>
+      </c>
+      <c r="D7">
+        <v>8</v>
       </c>
       <c r="E7" t="s">
         <v>6</v>
@@ -790,10 +821,13 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
+        <v>28</v>
+      </c>
+      <c r="D8">
+        <v>10</v>
       </c>
       <c r="E8" t="s">
         <v>6</v>
@@ -804,10 +838,13 @@
         <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C9" t="s">
-        <v>26</v>
+        <v>25</v>
+      </c>
+      <c r="D9">
+        <v>12</v>
       </c>
       <c r="E9" t="s">
         <v>6</v>
@@ -818,10 +855,13 @@
         <v>2</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C10" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="D10">
+        <v>14</v>
       </c>
       <c r="E10" t="s">
         <v>6</v>
@@ -832,7 +872,10 @@
         <v>2</v>
       </c>
       <c r="C11" t="s">
-        <v>33</v>
+        <v>32</v>
+      </c>
+      <c r="D11">
+        <v>20</v>
       </c>
       <c r="E11" t="s">
         <v>6</v>
@@ -843,10 +886,13 @@
         <v>2</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C12" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="D12">
+        <v>12</v>
       </c>
       <c r="E12" t="s">
         <v>6</v>
@@ -857,7 +903,10 @@
         <v>2</v>
       </c>
       <c r="C13" t="s">
-        <v>34</v>
+        <v>33</v>
+      </c>
+      <c r="D13">
+        <v>10</v>
       </c>
       <c r="E13" t="s">
         <v>6</v>
@@ -871,13 +920,19 @@
         <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>20</v>
+        <v>19</v>
+      </c>
+      <c r="D14">
+        <v>90</v>
       </c>
       <c r="E14" t="s">
         <v>12</v>
       </c>
+      <c r="F14" t="s">
+        <v>49</v>
+      </c>
       <c r="H14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
@@ -885,10 +940,13 @@
         <v>3</v>
       </c>
       <c r="B15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C15" t="s">
-        <v>30</v>
+        <v>29</v>
+      </c>
+      <c r="D15">
+        <v>12</v>
       </c>
       <c r="E15" t="s">
         <v>12</v>
@@ -899,604 +957,773 @@
         <v>3</v>
       </c>
       <c r="B16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C16" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+      <c r="D16">
+        <v>75</v>
       </c>
       <c r="E16" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F16" t="s">
+        <v>49</v>
+      </c>
+      <c r="H16" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>3</v>
       </c>
       <c r="C17" t="s">
-        <v>36</v>
+        <v>107</v>
       </c>
       <c r="E17" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C18" t="s">
-        <v>38</v>
+        <v>103</v>
+      </c>
+      <c r="D18">
+        <v>60</v>
       </c>
       <c r="E18" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+      <c r="F18" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>4</v>
       </c>
       <c r="C19" t="s">
-        <v>39</v>
+        <v>36</v>
+      </c>
+      <c r="D19">
+        <v>13</v>
       </c>
       <c r="E19" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>4</v>
       </c>
       <c r="C20" t="s">
-        <v>40</v>
+        <v>37</v>
+      </c>
+      <c r="D20">
+        <v>60</v>
       </c>
       <c r="E20" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F20" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>4</v>
       </c>
       <c r="C21" t="s">
-        <v>41</v>
+        <v>38</v>
+      </c>
+      <c r="D21">
+        <v>17</v>
       </c>
       <c r="E21" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>4</v>
       </c>
       <c r="C22" t="s">
-        <v>42</v>
+        <v>39</v>
+      </c>
+      <c r="D22">
+        <v>24</v>
       </c>
       <c r="E22" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F22" t="s">
+        <v>49</v>
+      </c>
+      <c r="H22" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>4</v>
       </c>
       <c r="C23" t="s">
-        <v>43</v>
+        <v>40</v>
+      </c>
+      <c r="D23">
+        <v>14</v>
       </c>
       <c r="E23" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>4</v>
       </c>
       <c r="C24" t="s">
-        <v>44</v>
+        <v>41</v>
+      </c>
+      <c r="D24">
+        <v>16</v>
       </c>
       <c r="E24" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>4</v>
       </c>
       <c r="C25" t="s">
+        <v>42</v>
+      </c>
+      <c r="D25">
+        <v>12</v>
+      </c>
+      <c r="E25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>5</v>
+      </c>
+      <c r="C26" t="s">
+        <v>43</v>
+      </c>
+      <c r="D26">
+        <v>24</v>
+      </c>
+      <c r="E26" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>5</v>
+      </c>
+      <c r="C27" t="s">
+        <v>44</v>
+      </c>
+      <c r="D27">
+        <v>36</v>
+      </c>
+      <c r="E27" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>5</v>
+      </c>
+      <c r="C28" t="s">
         <v>45</v>
       </c>
-      <c r="E25" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26">
-        <v>5</v>
-      </c>
-      <c r="C26" t="s">
+      <c r="D28">
+        <v>18</v>
+      </c>
+      <c r="E28" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>5</v>
+      </c>
+      <c r="C29" t="s">
         <v>46</v>
       </c>
-      <c r="E26" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27">
-        <v>5</v>
-      </c>
-      <c r="C27" t="s">
+      <c r="D29">
+        <v>17</v>
+      </c>
+      <c r="E29" t="s">
         <v>47</v>
       </c>
-      <c r="E27" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28">
-        <v>5</v>
-      </c>
-      <c r="C28" t="s">
+      <c r="G29" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>5</v>
+      </c>
+      <c r="C30" t="s">
+        <v>50</v>
+      </c>
+      <c r="D30">
+        <v>15</v>
+      </c>
+      <c r="E30" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>5</v>
+      </c>
+      <c r="C31" t="s">
+        <v>51</v>
+      </c>
+      <c r="D31">
+        <v>300</v>
+      </c>
+      <c r="E31" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>5</v>
+      </c>
+      <c r="C32" t="s">
+        <v>67</v>
+      </c>
+      <c r="D32">
+        <v>12</v>
+      </c>
+      <c r="E32" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>5</v>
+      </c>
+      <c r="C33" t="s">
+        <v>109</v>
+      </c>
+      <c r="D33">
+        <v>19</v>
+      </c>
+      <c r="E33" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>6</v>
+      </c>
+      <c r="C34" t="s">
+        <v>100</v>
+      </c>
+      <c r="D34">
+        <v>18</v>
+      </c>
+      <c r="E34" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>6</v>
+      </c>
+      <c r="C35" t="s">
+        <v>52</v>
+      </c>
+      <c r="D35">
+        <v>17</v>
+      </c>
+      <c r="E35" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>6</v>
+      </c>
+      <c r="C36" t="s">
+        <v>54</v>
+      </c>
+      <c r="D36">
+        <v>150</v>
+      </c>
+      <c r="E36" t="s">
+        <v>6</v>
+      </c>
+      <c r="F36" t="s">
+        <v>49</v>
+      </c>
+      <c r="H36" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>6</v>
+      </c>
+      <c r="C37" t="s">
+        <v>55</v>
+      </c>
+      <c r="D37">
+        <v>24</v>
+      </c>
+      <c r="E37" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>6</v>
+      </c>
+      <c r="C38" t="s">
+        <v>65</v>
+      </c>
+      <c r="D38">
+        <v>16</v>
+      </c>
+      <c r="E38" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>6</v>
+      </c>
+      <c r="C39" t="s">
+        <v>66</v>
+      </c>
+      <c r="D39">
+        <v>15</v>
+      </c>
+      <c r="E39" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>6</v>
+      </c>
+      <c r="C40" t="s">
+        <v>68</v>
+      </c>
+      <c r="D40">
+        <v>17</v>
+      </c>
+      <c r="E40" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>7</v>
+      </c>
+      <c r="C41" t="s">
+        <v>56</v>
+      </c>
+      <c r="D41">
         <v>48</v>
       </c>
-      <c r="E28" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29">
-        <v>5</v>
-      </c>
-      <c r="C29" t="s">
-        <v>49</v>
-      </c>
-      <c r="E29" t="s">
-        <v>50</v>
-      </c>
-      <c r="G29" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30">
-        <v>5</v>
-      </c>
-      <c r="C30" t="s">
-        <v>53</v>
-      </c>
-      <c r="E30" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31">
-        <v>5</v>
-      </c>
-      <c r="C31" t="s">
-        <v>54</v>
-      </c>
-      <c r="E31" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32">
-        <v>6</v>
-      </c>
-      <c r="C32" t="s">
-        <v>55</v>
-      </c>
-      <c r="E32" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33">
-        <v>6</v>
-      </c>
-      <c r="C33" t="s">
-        <v>56</v>
-      </c>
-      <c r="E33" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34">
-        <v>6</v>
-      </c>
-      <c r="C34" t="s">
+      <c r="E41" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>7</v>
+      </c>
+      <c r="C42" t="s">
+        <v>57</v>
+      </c>
+      <c r="D42">
+        <v>100</v>
+      </c>
+      <c r="E42" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>7</v>
+      </c>
+      <c r="C43" t="s">
         <v>58</v>
       </c>
-      <c r="E34" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35">
-        <v>6</v>
-      </c>
-      <c r="C35" t="s">
+      <c r="D43">
+        <v>21</v>
+      </c>
+      <c r="E43" t="s">
+        <v>47</v>
+      </c>
+      <c r="G43" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>7</v>
+      </c>
+      <c r="C44" t="s">
         <v>59</v>
       </c>
-      <c r="E35" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36">
+      <c r="D44">
+        <v>200</v>
+      </c>
+      <c r="E44" t="s">
+        <v>6</v>
+      </c>
+      <c r="F44" t="s">
+        <v>49</v>
+      </c>
+      <c r="H44" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A45">
         <v>7</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C45" t="s">
         <v>60</v>
       </c>
-      <c r="E36" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37">
-        <v>7</v>
-      </c>
-      <c r="C37" t="s">
+      <c r="D45">
+        <v>300</v>
+      </c>
+      <c r="E45" t="s">
         <v>61</v>
       </c>
-      <c r="E37" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38">
-        <v>7</v>
-      </c>
-      <c r="C38" t="s">
+      <c r="G45" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>8</v>
+      </c>
+      <c r="C46" t="s">
         <v>62</v>
       </c>
-      <c r="E38" t="s">
-        <v>50</v>
-      </c>
-      <c r="G38" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39">
-        <v>7</v>
-      </c>
-      <c r="C39" t="s">
+      <c r="D46">
+        <v>120</v>
+      </c>
+      <c r="E46" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>8</v>
+      </c>
+      <c r="C47" t="s">
+        <v>71</v>
+      </c>
+      <c r="D47">
+        <v>30</v>
+      </c>
+      <c r="E47" t="s">
+        <v>72</v>
+      </c>
+      <c r="G47" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>9</v>
+      </c>
+      <c r="C48" t="s">
+        <v>64</v>
+      </c>
+      <c r="D48">
+        <v>500</v>
+      </c>
+      <c r="E48" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>10</v>
+      </c>
+      <c r="C49" t="s">
         <v>63</v>
       </c>
-      <c r="E39" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A40">
-        <v>7</v>
-      </c>
-      <c r="C40" t="s">
-        <v>64</v>
-      </c>
-      <c r="E40" t="s">
-        <v>65</v>
-      </c>
-      <c r="G40" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41">
-        <v>8</v>
-      </c>
-      <c r="C41" t="s">
-        <v>66</v>
-      </c>
-      <c r="E41" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42">
-        <v>8</v>
-      </c>
-      <c r="C42" t="s">
+      <c r="D49">
+        <v>500</v>
+      </c>
+      <c r="E49" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>11</v>
+      </c>
+      <c r="C50" t="s">
+        <v>69</v>
+      </c>
+      <c r="D50">
+        <v>45</v>
+      </c>
+      <c r="E50" t="s">
+        <v>70</v>
+      </c>
+      <c r="G50" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C51" t="s">
+        <v>74</v>
+      </c>
+      <c r="E51" t="s">
+        <v>61</v>
+      </c>
+      <c r="G51" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C52" t="s">
+        <v>75</v>
+      </c>
+      <c r="E52" t="s">
+        <v>61</v>
+      </c>
+      <c r="G52" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C53" t="s">
         <v>76</v>
       </c>
-      <c r="E42" t="s">
+      <c r="E53" t="s">
+        <v>61</v>
+      </c>
+      <c r="G53" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C54" t="s">
         <v>77</v>
       </c>
-      <c r="G42" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43">
-        <v>9</v>
-      </c>
-      <c r="C43" t="s">
-        <v>68</v>
-      </c>
-      <c r="E43" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A44">
-        <v>10</v>
-      </c>
-      <c r="C44" t="s">
-        <v>67</v>
-      </c>
-      <c r="E44" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A45">
-        <v>11</v>
-      </c>
-      <c r="C45" t="s">
-        <v>74</v>
-      </c>
-      <c r="E45" t="s">
-        <v>75</v>
-      </c>
-      <c r="G45" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C46" t="s">
-        <v>69</v>
-      </c>
-      <c r="E46" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C47" t="s">
-        <v>70</v>
-      </c>
-      <c r="E47" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C48" t="s">
-        <v>71</v>
-      </c>
-      <c r="E48" t="s">
+      <c r="E54" t="s">
+        <v>61</v>
+      </c>
+      <c r="G54" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C55" t="s">
+        <v>78</v>
+      </c>
+      <c r="E55" t="s">
+        <v>61</v>
+      </c>
+      <c r="G55" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C56" t="s">
+        <v>79</v>
+      </c>
+      <c r="E56" t="s">
+        <v>61</v>
+      </c>
+      <c r="G56" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C57" t="s">
+        <v>80</v>
+      </c>
+      <c r="E57" t="s">
+        <v>61</v>
+      </c>
+      <c r="G57" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C58" t="s">
+        <v>81</v>
+      </c>
+      <c r="E58" t="s">
+        <v>61</v>
+      </c>
+      <c r="G58" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C59" t="s">
+        <v>82</v>
+      </c>
+      <c r="E59" t="s">
+        <v>61</v>
+      </c>
+      <c r="G59" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C60" t="s">
+        <v>83</v>
+      </c>
+      <c r="E60" t="s">
+        <v>61</v>
+      </c>
+      <c r="G60" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C61" t="s">
+        <v>84</v>
+      </c>
+      <c r="E61" t="s">
+        <v>61</v>
+      </c>
+      <c r="G61" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C62" t="s">
+        <v>85</v>
+      </c>
+      <c r="E62" t="s">
+        <v>61</v>
+      </c>
+      <c r="G62" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C63" t="s">
+        <v>86</v>
+      </c>
+      <c r="E63" t="s">
+        <v>89</v>
+      </c>
+      <c r="G63" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C64" t="s">
+        <v>87</v>
+      </c>
+      <c r="E64" t="s">
+        <v>89</v>
+      </c>
+      <c r="G64" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C65" t="s">
+        <v>88</v>
+      </c>
+      <c r="E65" t="s">
+        <v>89</v>
+      </c>
+      <c r="G65" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C66" t="s">
+        <v>90</v>
+      </c>
+      <c r="E66" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C67" t="s">
+        <v>92</v>
+      </c>
+      <c r="E67" t="s">
+        <v>93</v>
+      </c>
+      <c r="G67" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C68" t="s">
+        <v>94</v>
+      </c>
+      <c r="E68" t="s">
+        <v>96</v>
+      </c>
+      <c r="G68" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C69" t="s">
+        <v>90</v>
+      </c>
+      <c r="E69" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C70" t="s">
+        <v>95</v>
+      </c>
+      <c r="E70" t="s">
+        <v>96</v>
+      </c>
+      <c r="G70" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="C71" t="s">
+        <v>101</v>
+      </c>
+      <c r="E71" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="49" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C49" t="s">
-        <v>72</v>
-      </c>
-      <c r="E49" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="50" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C50" t="s">
-        <v>73</v>
-      </c>
-      <c r="E50" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="51" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C51" t="s">
-        <v>79</v>
-      </c>
-      <c r="E51" t="s">
-        <v>65</v>
-      </c>
-      <c r="G51" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="52" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C52" t="s">
-        <v>80</v>
-      </c>
-      <c r="E52" t="s">
-        <v>65</v>
-      </c>
-      <c r="G52" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="53" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C53" t="s">
-        <v>81</v>
-      </c>
-      <c r="E53" t="s">
-        <v>65</v>
-      </c>
-      <c r="G53" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="54" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C54" t="s">
-        <v>82</v>
-      </c>
-      <c r="E54" t="s">
-        <v>65</v>
-      </c>
-      <c r="G54" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="55" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C55" t="s">
-        <v>83</v>
-      </c>
-      <c r="E55" t="s">
-        <v>65</v>
-      </c>
-      <c r="G55" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="56" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C56" t="s">
-        <v>84</v>
-      </c>
-      <c r="E56" t="s">
-        <v>65</v>
-      </c>
-      <c r="G56" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="57" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C57" t="s">
-        <v>85</v>
-      </c>
-      <c r="E57" t="s">
-        <v>65</v>
-      </c>
-      <c r="G57" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="58" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C58" t="s">
-        <v>86</v>
-      </c>
-      <c r="E58" t="s">
-        <v>65</v>
-      </c>
-      <c r="G58" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="59" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C59" t="s">
-        <v>87</v>
-      </c>
-      <c r="E59" t="s">
-        <v>65</v>
-      </c>
-      <c r="G59" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="60" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C60" t="s">
-        <v>88</v>
-      </c>
-      <c r="E60" t="s">
-        <v>65</v>
-      </c>
-      <c r="G60" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="61" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C61" t="s">
-        <v>89</v>
-      </c>
-      <c r="E61" t="s">
-        <v>65</v>
-      </c>
-      <c r="G61" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="62" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C62" t="s">
-        <v>90</v>
-      </c>
-      <c r="E62" t="s">
-        <v>65</v>
-      </c>
-      <c r="G62" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="63" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C63" t="s">
-        <v>91</v>
-      </c>
-      <c r="E63" t="s">
-        <v>94</v>
-      </c>
-      <c r="G63" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="64" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C64" t="s">
-        <v>92</v>
-      </c>
-      <c r="E64" t="s">
-        <v>94</v>
-      </c>
-      <c r="G64" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="65" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C65" t="s">
-        <v>93</v>
-      </c>
-      <c r="E65" t="s">
-        <v>94</v>
-      </c>
-      <c r="G65" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="66" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C66" t="s">
-        <v>95</v>
-      </c>
-      <c r="E66" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="67" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C67" t="s">
-        <v>97</v>
-      </c>
-      <c r="E67" t="s">
-        <v>98</v>
-      </c>
-      <c r="G67" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="68" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C68" t="s">
-        <v>99</v>
-      </c>
-      <c r="E68" t="s">
-        <v>101</v>
-      </c>
-      <c r="G68" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="69" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C69" t="s">
-        <v>95</v>
-      </c>
-      <c r="E69" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="70" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C70" t="s">
-        <v>100</v>
-      </c>
-      <c r="E70" t="s">
-        <v>101</v>
-      </c>
-      <c r="G70" t="s">
-        <v>52</v>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <v>5</v>
+      </c>
+      <c r="C72" t="s">
+        <v>108</v>
+      </c>
+      <c r="E72" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G50">
+    <sortCondition ref="A2:A50"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>